<commit_message>
tomar valor de celda
</commit_message>
<xml_diff>
--- a/Estado de Resultados/Files/plantilla.xlsx
+++ b/Estado de Resultados/Files/plantilla.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gris8\OneDrive\Documentos\PRACTICAS PROFESIONALES\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gris8\OneDrive\Documentos\PRACTICAS PROFESIONALES\Dialogs\prueba\Estado-de-Resultados-Estad-a\Estado de Resultados\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F88F287F-EAE3-4AE5-8E18-1A8B061CD2FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB1BBB52-D3A4-4A32-81C9-A3BF78F4FFD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{DAF5CDE0-CF02-46E4-B639-F716AC9FA5E2}"/>
   </bookViews>
@@ -440,7 +440,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -462,11 +462,12 @@
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -907,7 +908,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -930,8 +931,8 @@
       <c r="A2" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="8">
+      <c r="B2" s="11"/>
+      <c r="C2" s="12">
         <f>Tabla4[[#Totals],[INGRESOS]]</f>
         <v>936727</v>
       </c>
@@ -940,10 +941,10 @@
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="12">
         <f>Tabla2[[#Totals],[GASTOS ADMINISTRATIVOS]]</f>
         <v>308316.28000000003</v>
       </c>
@@ -952,8 +953,8 @@
       <c r="A4" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="11">
+      <c r="B4" s="11"/>
+      <c r="C4" s="13">
         <f>C2-C3</f>
         <v>628410.72</v>
       </c>
@@ -962,10 +963,10 @@
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5" s="12">
         <f>Tabla1[[#Totals],[GASTOS OPERACIONALES]]</f>
         <v>120422.22</v>
       </c>
@@ -977,7 +978,7 @@
       <c r="B6" t="s">
         <v>100</v>
       </c>
-      <c r="C6" s="13">
+      <c r="C6" s="14">
         <f>C4-C5</f>
         <v>507988.5</v>
       </c>
@@ -986,10 +987,10 @@
       <c r="A7" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C7" s="12">
         <f>C6*0.3</f>
         <v>152396.54999999999</v>
       </c>
@@ -998,7 +999,7 @@
       <c r="A8" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="C8" s="8">
+      <c r="C8" s="12">
         <f>C6-C7</f>
         <v>355591.95</v>
       </c>

</xml_diff>